<commit_message>
seera and sample datasets and exploratory analysis
</commit_message>
<xml_diff>
--- a/Research_sources.xlsx
+++ b/Research_sources.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\offic\Documents\SIT723_T3\SIT723_T3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27CB48A7-64A4-4AAE-BFD5-2D571E918784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{387E02EE-1923-4421-B029-6411E9239005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="58">
   <si>
     <t>Titles</t>
   </si>
@@ -160,6 +160,54 @@
   </si>
   <si>
     <t>AIOps: Real-World Challenges and Research Innovations</t>
+  </si>
+  <si>
+    <t>SEERA: A software cost estimation dataset for constrained environments</t>
+  </si>
+  <si>
+    <t>(PDF) SEERA: A software cost estimation dataset for constrained environments (researchgate.net)</t>
+  </si>
+  <si>
+    <t>COCOMO (Constructive Cost Model) (immagic.com)</t>
+  </si>
+  <si>
+    <t>Constructive Cost Model (COCOMO)</t>
+  </si>
+  <si>
+    <t>(PDF) A Review of Machine Learning Models for Software Cost Estimation (researchgate.net)</t>
+  </si>
+  <si>
+    <t>A Review of Machine Learning Models for Software Cost Estimation</t>
+  </si>
+  <si>
+    <t>AI Doesn’t Have to Be Too Complicated or Expensive for Your Business</t>
+  </si>
+  <si>
+    <t>AI Doesn’t Have to Be Too Complicated or Expensive for Your Business (hbr.org)</t>
+  </si>
+  <si>
+    <t>Comparison and evaluation of data mining techniques with algorithmic models in software cost estimation - ScienceDirect</t>
+  </si>
+  <si>
+    <t>Comparison and evaluation of data mining techniques with algorithmic models in software cost estimation</t>
+  </si>
+  <si>
+    <t>Uncertainty calculation in life cycle assessments</t>
+  </si>
+  <si>
+    <t>Uncertainty calculation in life cycle assessments | SpringerLink</t>
+  </si>
+  <si>
+    <t>Estimation of Effort in Software Cost Analysis for Heterogenous Dataset using Fuzzy Analogy</t>
+  </si>
+  <si>
+    <t>[1211.1136] Estimation of Effort in Software Cost Analysis for Heterogenous Dataset using Fuzzy Analogy (arxiv.org)</t>
+  </si>
+  <si>
+    <t>Here are the different types of chatbots:</t>
+  </si>
+  <si>
+    <t>6 types of chatbots - Which is best for your business? (engati.com)</t>
   </si>
 </sst>
 </file>
@@ -231,7 +279,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -246,6 +294,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -315,8 +364,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A9E3416C-17BC-40CB-A48B-D26BADB3A7EA}" name="Table2" displayName="Table2" ref="A2:C21" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="A2:C21" xr:uid="{A9E3416C-17BC-40CB-A48B-D26BADB3A7EA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A9E3416C-17BC-40CB-A48B-D26BADB3A7EA}" name="Table2" displayName="Table2" ref="A2:C38" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A2:C38" xr:uid="{A9E3416C-17BC-40CB-A48B-D26BADB3A7EA}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{1E6A5819-020D-453A-8345-071C5F16F002}" name="Titles" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{A2EC14D7-BFB4-4E78-9EBA-F5CF6B430725}" name="Sources" dataDxfId="1" dataCellStyle="Hyperlink"/>
@@ -589,10 +638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -828,6 +877,189 @@
       <c r="C21" s="4" t="s">
         <v>31</v>
       </c>
+    </row>
+    <row r="22" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C37" s="4"/>
+    </row>
+    <row r="38" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C38" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -853,11 +1085,28 @@
     <hyperlink ref="B19" r:id="rId17" display="https://ieeexplore-ieee-org.ezproxy-f.deakin.edu.au/document/9492289" xr:uid="{C40BB220-465D-44FE-8270-5025F2EE8E8D}"/>
     <hyperlink ref="B20" r:id="rId18" display="https://ieeexplore-ieee-org.ezproxy-f.deakin.edu.au/document/5598114" xr:uid="{78EC58BB-AF11-4611-946F-7BADA651A094}"/>
     <hyperlink ref="B21" r:id="rId19" display="https://ieeexplore-ieee-org.ezproxy-f.deakin.edu.au/document/8802836" xr:uid="{7FB8CA4B-7323-45BB-9602-B2921C15731C}"/>
+    <hyperlink ref="B22" r:id="rId20" display="https://ieeexplore-ieee-org.ezproxy-f.deakin.edu.au/document/8724092" xr:uid="{AB5A555A-27D7-486A-9CFB-FDEACC88BA3A}"/>
+    <hyperlink ref="B23" r:id="rId21" display="https://ieeexplore-ieee-org.ezproxy-f.deakin.edu.au/document/9007411" xr:uid="{C15BA657-BBFA-4355-9357-475EA0FE2020}"/>
+    <hyperlink ref="B24" r:id="rId22" display="https://ieeexplore-ieee-org.ezproxy-f.deakin.edu.au/document/9056955" xr:uid="{E917CDB8-218D-4B48-8DE8-4E8ECB68D6D0}"/>
+    <hyperlink ref="B25" r:id="rId23" display="https://ieeexplore-ieee-org.ezproxy-f.deakin.edu.au/document/9007411" xr:uid="{C8CECE08-765A-4547-94C8-10F4FD330DFB}"/>
+    <hyperlink ref="B26" r:id="rId24" location="citations" display="https://ieeexplore-ieee-org.ezproxy-f.deakin.edu.au/document/1293068/citations - citations" xr:uid="{A670AEAB-ACD4-4744-90B9-65CA35B88C92}"/>
+    <hyperlink ref="B27" r:id="rId25" display="https://ieeexplore-ieee-org.ezproxy-f.deakin.edu.au/document/5173033" xr:uid="{52355E6C-1832-4029-ABB9-5ECF27A4900F}"/>
+    <hyperlink ref="B28" r:id="rId26" display="https://ieeexplore-ieee-org.ezproxy-f.deakin.edu.au/document/299437" xr:uid="{B7394FAD-F40B-4094-AF70-FEE712231E56}"/>
+    <hyperlink ref="B29" r:id="rId27" display="https://ieeexplore-ieee-org.ezproxy-f.deakin.edu.au/document/1293069" xr:uid="{B77099DA-D3EE-43C8-8C6C-245DD0FA1F3D}"/>
+    <hyperlink ref="B30" r:id="rId28" display="https://ieeexplore-ieee-org.ezproxy-f.deakin.edu.au/document/1293073" xr:uid="{5A5F84EB-7496-4F20-83A4-1BFA8CAEDF7B}"/>
+    <hyperlink ref="B31" r:id="rId29" display="https://www.researchgate.net/publication/346734027_SEERA_A_software_cost_estimation_dataset_for_constrained_environments" xr:uid="{910325E2-5EF4-4694-B5AE-293ECF33913F}"/>
+    <hyperlink ref="B32" r:id="rId30" display="https://www.immagic.com/eLibrary/ARCHIVES/GENERAL/WIKIPEDI/W120626C.pdf" xr:uid="{19E10717-9C2E-4C57-9CBE-F9B9C4A1EF9B}"/>
+    <hyperlink ref="B33" r:id="rId31" display="https://www.researchgate.net/publication/337243523_A_Review_of_Machine_Learning_Models_for_Software_Cost_Estimation" xr:uid="{898924F7-803D-4F05-A0FB-DB2089E251F0}"/>
+    <hyperlink ref="B34" r:id="rId32" display="https://hbr.org/2021/07/ai-doesnt-have-to-be-too-complicated-or-expensive-for-your-business" xr:uid="{90550C10-7B43-49D6-86AC-9CE8BFDC3F1B}"/>
+    <hyperlink ref="B35" r:id="rId33" display="https://www.sciencedirect.com/science/article/pii/S221201731200014X" xr:uid="{510258C5-DDAF-4B02-A903-A29C6674EF15}"/>
+    <hyperlink ref="B36" r:id="rId34" display="https://link.springer.com/article/10.1007/BF02978597" xr:uid="{1D2D8990-1715-40C4-95FE-1786B0F2E8C1}"/>
+    <hyperlink ref="B37" r:id="rId35" display="https://arxiv.org/abs/1211.1136" xr:uid="{008AFF4C-C615-40F7-A022-A665A3054A8D}"/>
+    <hyperlink ref="B38" r:id="rId36" display="https://www.engati.com/blog/types-of-chatbots-and-their-applications?utm_content=types-of-chatbots-and-their-applications" xr:uid="{7342A957-F78D-4BDE-AF5A-3B064F14CE02}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId20"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId37"/>
   <tableParts count="1">
-    <tablePart r:id="rId21"/>
+    <tablePart r:id="rId38"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>